<commit_message>
enhance phone number extraction logic in transfer between branches form
</commit_message>
<xml_diff>
--- a/transfer/public/asset/xlsx/Account111.xlsx
+++ b/transfer/public/asset/xlsx/Account111.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="150">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -50,8 +50,50 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1000 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">خزنة غريان </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- A</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">خزنة غريان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LYD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">الفروع </t>
     </r>
@@ -67,52 +109,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">الفروع</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LYD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cash In Hand - A</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1000 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">خزنة غريان </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- A</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">خزنة غريان</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cash</t>
   </si>
   <si>
@@ -132,6 +128,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة ابوسليم </t>
     </r>
@@ -169,6 +166,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية الكفرة </t>
     </r>
@@ -206,6 +204,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية بن جواد </t>
     </r>
@@ -243,6 +242,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية اجدابيا </t>
     </r>
@@ -280,6 +280,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية زليتن </t>
     </r>
@@ -317,6 +318,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية مصراته </t>
     </r>
@@ -354,6 +356,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية الزاوية </t>
     </r>
@@ -391,6 +394,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية سرت </t>
     </r>
@@ -428,6 +432,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية صبراته </t>
     </r>
@@ -465,6 +470,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية سوق الاحد </t>
     </r>
@@ -502,6 +508,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية بني وليد </t>
     </r>
@@ -539,6 +546,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية الخمس </t>
     </r>
@@ -576,6 +584,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية وادي الربيع </t>
     </r>
@@ -613,6 +622,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">خزنة العالمية الفرناج </t>
     </r>
@@ -638,8 +648,47 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2000 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">عمولات غريان </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- A</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">عمولات غريان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات </t>
     </r>
@@ -655,49 +704,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">عمولات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direct Income - A</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2000 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">عمولات غريان </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- A</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">عمولات غريان</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Direct Income</t>
   </si>
   <si>
@@ -717,6 +723,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات ابوسليم </t>
     </r>
@@ -757,6 +764,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية الكفرة </t>
     </r>
@@ -794,6 +802,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية بن جواد </t>
     </r>
@@ -831,6 +840,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية اجدابيا </t>
     </r>
@@ -868,6 +878,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية زليتن </t>
     </r>
@@ -905,6 +916,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية مصراته </t>
     </r>
@@ -942,6 +954,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية الزاوية </t>
     </r>
@@ -979,6 +992,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية سرت </t>
     </r>
@@ -1016,6 +1030,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية صبراته </t>
     </r>
@@ -1053,6 +1068,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية سوق الاحد </t>
     </r>
@@ -1090,6 +1106,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية بني وليد </t>
     </r>
@@ -1127,6 +1144,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية الخمس </t>
     </r>
@@ -1164,6 +1182,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية وادي الربيع </t>
     </r>
@@ -1201,6 +1220,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">عمولات العالمية الفرناج </t>
     </r>
@@ -1226,8 +1246,47 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3000 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">معلقات غريان </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- A</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">معلقات غريان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات </t>
     </r>
@@ -1243,49 +1302,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">معلقات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current Liabilities - A</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">3000 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">معلقات غريان </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- A</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">معلقات غريان</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3000</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1302,6 +1318,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات ابوسليم </t>
     </r>
@@ -1339,6 +1356,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية الكفرة </t>
     </r>
@@ -1376,6 +1394,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية بن جواد </t>
     </r>
@@ -1413,6 +1432,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية اجدابيا </t>
     </r>
@@ -1450,6 +1470,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية زليتن </t>
     </r>
@@ -1487,6 +1508,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية مصراته </t>
     </r>
@@ -1524,6 +1546,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية الزاوية </t>
     </r>
@@ -1561,6 +1584,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية سرت </t>
     </r>
@@ -1598,6 +1622,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية صبراته </t>
     </r>
@@ -1635,6 +1660,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية سوق الاحد </t>
     </r>
@@ -1672,6 +1698,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية بني وليد </t>
     </r>
@@ -1709,6 +1736,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية الخمس </t>
     </r>
@@ -1746,6 +1774,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية وادي الربيع </t>
     </r>
@@ -1783,6 +1812,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">معلقات العالمية الفرناج </t>
     </r>
@@ -1846,6 +1876,7 @@
       <color theme="1"/>
       <name val="Noto Sans Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1890,16 +1921,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2095,1366 +2130,1217 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.76"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="0" t="n">
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="0" t="n">
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="n">
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="0" t="n">
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="0" t="n">
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="0" t="n">
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="0" t="n">
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="0" t="n">
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="B17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="0" t="n">
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="G18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="B20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" s="0" t="n">
+      <c r="B21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="0" t="n">
+      <c r="B22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="0" t="n">
+      <c r="B23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" s="0" t="n">
+      <c r="B24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" s="0" t="n">
+      <c r="B25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" s="0" t="n">
+      <c r="B26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H27" s="0" t="n">
+      <c r="B27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="0" t="n">
+      <c r="B28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="0" t="n">
+      <c r="B29" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="0" t="n">
+      <c r="B30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" s="0" t="n">
+      <c r="B31" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H32" s="0" t="n">
+      <c r="B32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="A33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="0" t="n">
+      <c r="G33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="0" t="n">
+      <c r="A34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="0" t="n">
+      <c r="A35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="0" t="n">
+      <c r="A36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="0" t="n">
+      <c r="A37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H38" s="0" t="n">
+      <c r="A38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="0" t="n">
+      <c r="A39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="0" t="n">
+      <c r="A40" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="0" t="n">
+      <c r="A41" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="0" t="n">
+      <c r="A42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="0" t="n">
+      <c r="A43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" s="0" t="n">
+      <c r="A44" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="0" t="n">
+      <c r="A45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>